<commit_message>
Losfahren nach Haltestelle ermöglichen (in Arbeit)
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\PycharmProjects\Bachelorarbeit_Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B01E84-3BEE-4253-8F05-77D172C29EDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59E6275-CABE-4BC3-A5DC-A013A08A5E44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -380,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0BB4CFC-4877-4FD6-BF56-167E70887CDC}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -481,7 +481,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>7.3</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="B6" s="2">
         <v>50</v>
@@ -498,10 +498,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <v>8</v>
+        <v>7.3</v>
       </c>
       <c r="B7" s="2">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C7" s="2">
         <v>0</v>
@@ -510,15 +510,15 @@
         <v>0</v>
       </c>
       <c r="E7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>9.1</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C8" s="2">
         <v>0</v>
@@ -527,23 +527,40 @@
         <v>0</v>
       </c>
       <c r="E8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
+        <v>9.1</v>
+      </c>
+      <c r="B9" s="2">
+        <v>50</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
         <v>9.1999999999999993</v>
       </c>
-      <c r="B9" s="2">
-        <v>50</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2">
+      <c r="B10" s="2">
+        <v>50</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Erweiterung der Outputdatei: Status
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\PycharmProjects\Bachelorarbeit_Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59E6275-CABE-4BC3-A5DC-A013A08A5E44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0A65B8-88B8-4B29-8B26-CDAED584051E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <t>Bushaltestelle?</t>
   </si>
   <si>
-    <t>Ampel/Kreuzung?</t>
+    <t>Ampel?</t>
   </si>
 </sst>
 </file>
@@ -383,7 +383,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -439,7 +439,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
@@ -456,7 +456,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
@@ -473,7 +473,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
@@ -484,13 +484,13 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B6" s="2">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2">
         <v>0</v>
       </c>
       <c r="D6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
@@ -507,7 +507,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="2">
         <v>0</v>
@@ -524,7 +524,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="2">
         <v>1</v>
@@ -541,7 +541,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
@@ -558,7 +558,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Sicherung vor Änderung SoC
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\PycharmProjects\Bachelorarbeit_Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D243E7EC-9DAC-4DEF-B571-0D5CADD2F84B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BD3E8C-C8F0-4584-BE0E-CE261148633F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -383,7 +383,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -456,7 +456,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
@@ -490,7 +490,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
@@ -507,7 +507,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="2">
         <v>0</v>
@@ -524,7 +524,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="2">
         <v>0</v>
@@ -541,7 +541,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
@@ -558,7 +558,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="2">
         <v>0</v>
@@ -575,7 +575,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Fehler mit SoC>100% korrigiert
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\PycharmProjects\Bachelorarbeit_Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BD3E8C-C8F0-4584-BE0E-CE261148633F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3049F9-8248-4CCA-89F6-D2F01805F2F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -383,7 +383,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -456,7 +456,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
@@ -490,7 +490,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
@@ -507,7 +507,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="2">
         <v>0</v>
@@ -524,7 +524,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="2">
         <v>0</v>
@@ -541,7 +541,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
@@ -558,7 +558,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="2">
         <v>0</v>
@@ -575,7 +575,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
KeyError Ursache (Inputdatei) gefunden
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\PycharmProjects\Bachelorarbeit_Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E2E6FB-A46E-4FC0-AED3-5AFE3D1A0CAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85327078-93CB-4FDB-887D-1FDEA9B7AA62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>zurückgelegte Distanz [km]</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Ampel?</t>
-  </si>
-  <si>
-    <t>6t</t>
   </si>
 </sst>
 </file>
@@ -383,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0BB4CFC-4877-4FD6-BF56-167E70887CDC}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -584,11 +581,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>